<commit_message>
update finding most larges substrings on text
</commit_message>
<xml_diff>
--- a/contratos.xlsx
+++ b/contratos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I31"/>
+  <dimension ref="A1:I48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1890,6 +1890,805 @@
         </is>
       </c>
     </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>033/2024</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>003/2023</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Não informado</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>07 de agosto de 2024</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>RABELLO CONSTRUÇÕES LTDA, CNPJ 26.695.883/0001-95</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>Tomada de Preços</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>Execução da obra da segunda etapa da requalificação da orla fluvial do Rio das Almas, na Sede do Município de Nilo Peçanha BA.</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>PREFEITURA MUNICIPAL DE NILO PEÇANHA – BA.</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>R$ 637.919,93 (Seiscentos e trinta e sete mil, novecentos e dezanove reais e noventa e três centavos).</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>033/2024</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>003/2023</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Não informado</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>07 de agosto de 2024</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>RABELLO CONSTRUÇÕES LTDA., CNPJ 26.695.883/0001-95</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>Tomada de Preços</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>"seleção de proposta mais vantajosa para Execução da obra da segunda etapa da requalificação da orla fluvial do Rio das Almas, na Sede do Município de Nilo Peçanha BA.", consoante às condições estabelecidas no edital da Tomada de Preços Nº 003/2023.</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>MUNICÍPIO DE NILO PEÇANHA, Estado da Bahia</t>
+        </is>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>R$ 637.919,93 (Seiscentos e trinta e sete mil, novecentos e dezanove reais e noventa e três centavos).</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>033/2024</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>003/2023</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Não informado</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>07 de agosto de 2024</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>RABELLO CONSTRUÇÕES LTDA., CNPJ 26.695.883/0001-95</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>Tomada de Preços</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>"seleção de proposta mais vantajosa para Execução da obra da segunda etapa da requalificação da orla fluvial do Rio das Almas, na Sede do Município de Nilo Peçanha BA.", consoante às condições estabelecidas no edital da Tomada de Preços Nº 003/2023.</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>MUNICÍPIO DE NILO PEÇANHA, CNPJ/MF N° 13.758.313/0001-55</t>
+        </is>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>R$ 637.919,93 (Seiscentos e trinta e sete mil, novecentos e dezanove reais e noventa e três centavos)</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>033/2024</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>003/2023</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Não informado</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>07 de agosto de 2024</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>RABELLO CONSTRUÇÕES LTDA., CNPJ 26.695.883/0001-95</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>Tomada de Preços</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>Execução da obra da segunda etapa da requalificação da orla fluvial do Rio das Almas, na Sede do Município de Nilo Peçanha BA.</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>MUNICÍPIO DE NILO PEÇANHA, CNPJ/MF N° 13.758.313/0001-55</t>
+        </is>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>R$ 637.919,93 (Seiscentos e trinta e sete mil, novecentos e dezanove reais e noventa e três centavos)</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>033/2024</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>003/2023</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Não informado</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>07 de agosto de 2024</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>RABELLO CONSTRUÇÕES LTDA., CNPJ 26.695.883/0001-95</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>Tomada de Preços</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>Execução da obra da segunda etapa da requalificação da orla fluvial do Rio das Almas, na Sede do Município de Nilo Peçanha BA.</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>MUNICÍPIO DE NILO PEÇANHA</t>
+        </is>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>R$ 637.919,93 (Seiscentos e trinta e sete mil, novecentos e dezanove reais e noventa e três centavos)</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>033/2024</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>003/2023</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Não informado</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>07 de agosto de 2024</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>RABELLO CONSTRUÇÕES LTDA., CNPJ 26.695.883/0001-95</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>Tomada de Preços</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>Execução da obra da segunda etapa da requalificação da orla fluvial do Rio das Almas, na Sede do Município de Nilo Peçanha BA.</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>MUNICÍPIO DE NILO PEÇANHA, CNPJ/MF N° 13.758.313/0001-55</t>
+        </is>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>R$ 637.919,93 (Seiscentos e trinta e sete mil, novecentos e dezanove reais e noventa e três centavos)</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>033/2024</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>003/2023</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Não informado</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>07 de agosto de 2024</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>RABELLO CONSTRUÇÕES LTDA., CNPJ 26.695.883/0001-95</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>Tomada de Preços</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>"seleção de proposta mais vantajosa para Execução da obra da segunda etapa da requalificação da orla fluvial do Rio das Almas, na Sede do Município de Nilo Peçanha BA.", consoante às condições estabelecidas no edital da Tomada de Preços Nº 003/2023.</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>MUNICÍPIO DE NILO PEÇANHA, CNPJ/MF N° 13.758.313/0001-55</t>
+        </is>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>R$ 637.919,93 (Seiscentos e trinta e sete mil, novecentos e dezanove reais e noventa e três centavos).</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>033/2024</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>003/2023</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Não informado</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>07 de agosto de 2024</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>RABELLO CONSTRUÇÕES LTDA., CNPJ 26.695.883/0001-95</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>Tomada de Preços</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>Execução da obra da segunda etapa da requalificação da orla fluvial do Rio das Almas, na Sede do Município de Nilo Peçanha BA.</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>MUNICÍPIO DE NILO PEÇANHA, CNPJ/MF N° 13.758.313/0001-55</t>
+        </is>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>R$ 637.919,93 (Seiscentos e trinta e sete mil, novecentos e dezanove reais e noventa e três centavos)</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>033/2024</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>003/2023</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Não informado</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>07 de agosto de 2024</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>RABELLO CONSTRUÇÕES LTDA., CNPJ 26.695.883/0001-95</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>Tomada de Preços</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>Execução da obra da segunda etapa da requalificação da orla fluvial do Rio das Almas, na Sede do Município de Nilo Peçanha BA.</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>MUNICÍPIO DE NILO PEÇANHA, CNPJ/MF N° 13.758.313/0001-55</t>
+        </is>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>R$ 637.919,93 (Seiscentos e trinta e sete mil, novecentos e dezanove reais e noventa e três centavos).</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>033/2024</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>003/2023</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Não informado</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>07 de agosto de 2024</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>RABELLO CONSTRUÇÕES LTDA., CNPJ 26.695.883/0001-95</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>Tomada de Preços</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>Execução da obra da segunda etapa da requalificação da orla fluvial do Rio das Almas, na Sede do Município de Nilo Peçanha BA.</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>MUNICÍPIO DE NILO PEÇANHA, Estado da Bahia</t>
+        </is>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>R$ 637.919,93 (Seiscentos e trinta e sete mil, novecentos e dezanove reais e noventa e três centavos)</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>033/2024</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>003/2023</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Não informado</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>07 de agosto de 2024</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>RABELLO CONSTRUÇÕES LTDA., CNPJ 26.695.883/0001-95</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>Tomada de Preços</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>Execução da obra da segunda etapa da requalificação da orla fluvial do Rio das Almas, na Sede do Município de Nilo Peçanha BA.</t>
+        </is>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>MUNICÍPIO DE NILO PEÇANHA, Estado da Bahia</t>
+        </is>
+      </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>R$ 637.919,93 (Seiscentos e trinta e sete mil, novecentos e dezanove reais e noventa e três centavos).</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>033/2024</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>003/2023</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Não informado</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>07 de agosto de 2024</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>RABELLO CONSTRUÇÕES LTDA., CNPJ 26.695.883/0001-95</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>Tomada de Preços</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>Execução da obra da segunda etapa da requalificação da orla fluvial do Rio das Almas, na Sede do Município de Nilo Peçanha BA.</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>MUNICÍPIO DE NILO PEÇANHA, Estado da Bahia</t>
+        </is>
+      </c>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>R$ 637.919,93 (Seiscentos e trinta e sete mil, novecentos e dezanove reais e noventa e três centavos)</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>033/2024</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>003/2023</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Não informado</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>07 de agosto de 2024</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>RABELLO CONSTRUÇÕES LTDA., CNPJ 26.695.883/0001-95</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>Tomada de Preços</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>Execução da obra da segunda etapa da requalificação da orla fluvial do Rio das Almas, na Sede do Município de Nilo Peçanha BA.</t>
+        </is>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>MUNICÍPIO DE NILO PEÇANHA</t>
+        </is>
+      </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>R$ 637.919,93 (Seiscentos e trinta e sete mil, novecentos e dezanove reais e noventa e três centavos).</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>033/2024</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>003/2023</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Não informado</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>07 de agosto de 2024</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>RABELLO CONSTRUÇÕES LTDA., CNPJ 26.695.883/0001-95</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>Tomada de Preços</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>"seleção de proposta mais vantajosa para Execução da obra da segunda etapa da requalificação da orla fluvial do Rio das Almas, na Sede do Município de Nilo Peçanha BA.", consoante às condições estabelecidas no edital da Tomada de Preços Nº 003/2023.</t>
+        </is>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>MUNICÍPIO DE NILO PEÇANHA, Estado da Bahia</t>
+        </is>
+      </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>R$ 637.919,93 (Seiscentos e trinta e sete mil, novecentos e dezanove reais e noventa e três centavos).</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>033/2024</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>003/2023</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Não informado</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>07 de agosto de 2024</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>RABELLO CONSTRUÇÕES LTDA., CNPJ 26.695.883/0001-95</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>Tomada de Preços</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>Execução da obra da segunda etapa da requalificação da orla fluvial do Rio das Almas, na Sede do Município de Nilo Peçanha BA.</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>MUNICÍPIO DE NILO PEÇANHA, Estado da Bahia</t>
+        </is>
+      </c>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>R$ 637.919,93 (Seiscentos e trinta e sete mil, novecentos e dezanove reais e noventa e três centavos)</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>033/2024</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>003/2023</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Não informado</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>07 de agosto de 2024</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>RABELLO CONSTRUÇÕES LTDA., CNPJ 26.695.883/0001-95</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>Tomada de Preços</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>Execução da obra da segunda etapa da requalificação da orla fluvial do Rio das Almas, na Sede do Município de Nilo Peçanha BA.</t>
+        </is>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>MUNICÍPIO DE NILO PEÇANHA, Estado da Bahia</t>
+        </is>
+      </c>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>R$ 637.919,93 (Seiscentos e trinta e sete mil, novecentos e dezanove reais e noventa e três centavos)</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>033/2024</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>003/2023</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Não informado</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>07 de agosto de 2024</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>RABELLO CONSTRUÇÕES LTDA., CNPJ 26.695.883/0001-95</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>Tomada de Preços</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>Execução da obra da segunda etapa da requalificação da orla fluvial do Rio das Almas, na Sede do Município de Nilo Peçanha BA.</t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>MUNICÍPIO DE NILO PEÇANHA, Estado da Bahia, pessoa jurídica de direito público interno, inscrita no CNPJ/MF N° 13.758.313/0001-55, situada na Rua Raimundo Brito, s/nº, centro, СЕР. 45.440-000, na cidade de Nilo Peçanha-Ba., fone (73) 3257-2434</t>
+        </is>
+      </c>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>R$ 637.919,93 (Seiscentos e trinta e sete mil, novecentos e dezanove reais e noventa e três centavos)</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
estabilizando aplicacao to deploy
</commit_message>
<xml_diff>
--- a/contratos.xlsx
+++ b/contratos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I48"/>
+  <dimension ref="A1:J72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -479,6 +479,11 @@
           <t>Valor do contrato</t>
         </is>
       </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>CNPJ</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -526,6 +531,7 @@
           <t>R$ 180.000,00 (cento e oitenta mil reais)</t>
         </is>
       </c>
+      <c r="J2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -573,6 +579,7 @@
           <t>R$ 22.496,00 (Vinte e dois mil quatrocentos e noventa e seis reais)</t>
         </is>
       </c>
+      <c r="J3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -620,6 +627,7 @@
           <t>R$ 22.496,00 (Vinte e dois mil quatrocentos e noventa e seis reais)</t>
         </is>
       </c>
+      <c r="J4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -667,6 +675,7 @@
           <t>R$ 180.000,00 (cento e oitenta mil reais)</t>
         </is>
       </c>
+      <c r="J5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -714,6 +723,7 @@
           <t>R$ 130.000,00 (cento e trinta mil reais)</t>
         </is>
       </c>
+      <c r="J6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -761,6 +771,7 @@
           <t>R$ 56.400,00</t>
         </is>
       </c>
+      <c r="J7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -808,6 +819,7 @@
           <t>R$ 56.400,00</t>
         </is>
       </c>
+      <c r="J8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -855,6 +867,7 @@
           <t>R$ 637.919,93 (Seiscentos e trinta e sete mil, novecentos e dezanove reais e noventa e três centavos).</t>
         </is>
       </c>
+      <c r="J9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -902,6 +915,7 @@
           <t>R$ 37.000,00 (trinta e sete mil reais)</t>
         </is>
       </c>
+      <c r="J10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -949,6 +963,7 @@
           <t>R$ 37.000,00 (trinta e sete mil reais)</t>
         </is>
       </c>
+      <c r="J11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -996,6 +1011,7 @@
           <t>R$ 56.400,00</t>
         </is>
       </c>
+      <c r="J12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1043,6 +1059,7 @@
           <t>R$ 130.000,00 (cento e trinta mil reais)</t>
         </is>
       </c>
+      <c r="J13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1090,6 +1107,7 @@
           <t>R$ 130.000,00 (cento e trinta mil reais)</t>
         </is>
       </c>
+      <c r="J14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1137,6 +1155,7 @@
           <t>Não informado</t>
         </is>
       </c>
+      <c r="J15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1184,6 +1203,7 @@
           <t>R$ 130.000,00 (cento e trinta mil reais)</t>
         </is>
       </c>
+      <c r="J16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1231,6 +1251,7 @@
           <t>R$ 130.000,00 (cento e trinta mil reais)</t>
         </is>
       </c>
+      <c r="J17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1278,6 +1299,7 @@
           <t>R$ 130.000,00 (cento e trinta mil reais)</t>
         </is>
       </c>
+      <c r="J18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1325,6 +1347,7 @@
           <t>R$ 130.000,00 (cento e trinta mil reais)</t>
         </is>
       </c>
+      <c r="J19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1372,6 +1395,7 @@
           <t>R$ 130.000,00 (cento e trinta mil reais)</t>
         </is>
       </c>
+      <c r="J20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1419,6 +1443,7 @@
           <t>R$ 22.496,00 (Vinte e dois mil quatrocentos e noventa e seis reais)</t>
         </is>
       </c>
+      <c r="J21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1466,6 +1491,7 @@
           <t>R$ 56.400,00</t>
         </is>
       </c>
+      <c r="J22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1513,6 +1539,7 @@
           <t>R$ 180.000,00 (cento e oitenta mil reais)</t>
         </is>
       </c>
+      <c r="J23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1560,6 +1587,7 @@
           <t>R$ 22.496,00 (Vinte e dois mil quatrocentos e noventa e seis reais)</t>
         </is>
       </c>
+      <c r="J24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1607,6 +1635,7 @@
           <t>R$ 22.496,00 (Vinte e dois mil quatrocentos e noventa e seis reais)</t>
         </is>
       </c>
+      <c r="J25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1654,6 +1683,7 @@
           <t>R$ 22.496,00 (Vinte e dois mil quatrocentos e noventa e seis reais)</t>
         </is>
       </c>
+      <c r="J26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1701,6 +1731,7 @@
           <t>R$ 22.496,00 (Vinte e dois mil quatrocentos e noventa e seis reais)</t>
         </is>
       </c>
+      <c r="J27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1748,6 +1779,7 @@
           <t>R$ 22.496,00 (Vinte e dois mil quatrocentos e noventa e seis reais)</t>
         </is>
       </c>
+      <c r="J28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1795,6 +1827,7 @@
           <t>R$ 22.496,00 (Vinte e dois mil quatrocentos e noventa e seis reais)</t>
         </is>
       </c>
+      <c r="J29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1842,6 +1875,7 @@
           <t>R$ 22.496,00 (Vinte e dois mil quatrocentos e noventa e seis reais)</t>
         </is>
       </c>
+      <c r="J30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1889,6 +1923,7 @@
           <t>R$ 130.000,00 (cento e trinta mil reais)</t>
         </is>
       </c>
+      <c r="J31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -1936,6 +1971,7 @@
           <t>R$ 637.919,93 (Seiscentos e trinta e sete mil, novecentos e dezanove reais e noventa e três centavos).</t>
         </is>
       </c>
+      <c r="J32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -1983,6 +2019,7 @@
           <t>R$ 637.919,93 (Seiscentos e trinta e sete mil, novecentos e dezanove reais e noventa e três centavos).</t>
         </is>
       </c>
+      <c r="J33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -2030,6 +2067,7 @@
           <t>R$ 637.919,93 (Seiscentos e trinta e sete mil, novecentos e dezanove reais e noventa e três centavos)</t>
         </is>
       </c>
+      <c r="J34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -2077,6 +2115,7 @@
           <t>R$ 637.919,93 (Seiscentos e trinta e sete mil, novecentos e dezanove reais e noventa e três centavos)</t>
         </is>
       </c>
+      <c r="J35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -2124,6 +2163,7 @@
           <t>R$ 637.919,93 (Seiscentos e trinta e sete mil, novecentos e dezanove reais e noventa e três centavos)</t>
         </is>
       </c>
+      <c r="J36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -2171,6 +2211,7 @@
           <t>R$ 637.919,93 (Seiscentos e trinta e sete mil, novecentos e dezanove reais e noventa e três centavos)</t>
         </is>
       </c>
+      <c r="J37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -2218,6 +2259,7 @@
           <t>R$ 637.919,93 (Seiscentos e trinta e sete mil, novecentos e dezanove reais e noventa e três centavos).</t>
         </is>
       </c>
+      <c r="J38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -2265,6 +2307,7 @@
           <t>R$ 637.919,93 (Seiscentos e trinta e sete mil, novecentos e dezanove reais e noventa e três centavos)</t>
         </is>
       </c>
+      <c r="J39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -2312,6 +2355,7 @@
           <t>R$ 637.919,93 (Seiscentos e trinta e sete mil, novecentos e dezanove reais e noventa e três centavos).</t>
         </is>
       </c>
+      <c r="J40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -2359,6 +2403,7 @@
           <t>R$ 637.919,93 (Seiscentos e trinta e sete mil, novecentos e dezanove reais e noventa e três centavos)</t>
         </is>
       </c>
+      <c r="J41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -2406,6 +2451,7 @@
           <t>R$ 637.919,93 (Seiscentos e trinta e sete mil, novecentos e dezanove reais e noventa e três centavos).</t>
         </is>
       </c>
+      <c r="J42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -2453,6 +2499,7 @@
           <t>R$ 637.919,93 (Seiscentos e trinta e sete mil, novecentos e dezanove reais e noventa e três centavos)</t>
         </is>
       </c>
+      <c r="J43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -2500,6 +2547,7 @@
           <t>R$ 637.919,93 (Seiscentos e trinta e sete mil, novecentos e dezanove reais e noventa e três centavos).</t>
         </is>
       </c>
+      <c r="J44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -2547,6 +2595,7 @@
           <t>R$ 637.919,93 (Seiscentos e trinta e sete mil, novecentos e dezanove reais e noventa e três centavos).</t>
         </is>
       </c>
+      <c r="J45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -2594,6 +2643,7 @@
           <t>R$ 637.919,93 (Seiscentos e trinta e sete mil, novecentos e dezanove reais e noventa e três centavos)</t>
         </is>
       </c>
+      <c r="J46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -2641,6 +2691,7 @@
           <t>R$ 637.919,93 (Seiscentos e trinta e sete mil, novecentos e dezanove reais e noventa e três centavos)</t>
         </is>
       </c>
+      <c r="J47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -2686,6 +2737,1192 @@
       <c r="I48" t="inlineStr">
         <is>
           <t>R$ 637.919,93 (Seiscentos e trinta e sete mil, novecentos e dezanove reais e noventa e três centavos)</t>
+        </is>
+      </c>
+      <c r="J48" t="inlineStr"/>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>067/2024</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>DV004/2024SEMAD</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>24 de maio de 2024</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>31 de dezembro de 2024</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>MARIA DE LOURDES MEIRELLES LISBOA DE BRITO, CNPJ 18.967.907/0001-90</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>DISPENSA DE LICITAÇÃO</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>Contratação de pessoa jurídica para prestação de serviços de locação, instalação e operação de equipamento tipo "GRID Box Truss e Portal" para utilização nos eventos do Município de Nilo Peçanha - BA., na forma estabelecida no Termo de Referência e de acordo com a proposta do contratado que para todos os efeitos integra este contrato como se transcrita fosse, apresentada na forma de anexo único ao presente.</t>
+        </is>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>PREFEITURA MUNICIPAL DE NILO PEÇANHA</t>
+        </is>
+      </c>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>56.400,00</t>
+        </is>
+      </c>
+      <c r="J49" t="inlineStr"/>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>067/2024</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Não informado</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>24 de maio de 2024</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>31 de dezembro de 2024</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>MARIA DE LOURDES MEIRELLES LISBOA DE BRITO, CNPJ 18.967.907/0001-90</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>DISPENSA DE LICITAÇÃO</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>Contratação de pessoa jurídica para prestação de serviços de locação, instalação e operação de equipamento tipo "GRID Box Truss e Portal" para utilização nos eventos do Município de Nilo Peçanha - BA., na forma estabelecida no Termo de Referência e de acordo com a proposta do contratado que para todos os efeitos integra este contrato como se transcrita fosse, apresentada na forma de anexo único ao presente.</t>
+        </is>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>PREFEITURA MUNICIPAL DE NILO PEÇANHA</t>
+        </is>
+      </c>
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>56.400,00</t>
+        </is>
+      </c>
+      <c r="J50" t="inlineStr"/>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>067/2024</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Não informado</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>24 de maio de 2024</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>Não informado</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>MARIA DE LOURDES MEIRELLES LISBOA DE BRITO, CNPJ 18.967.907/0001-90</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>DISPENSA DE LICITAÇÃO</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>Contratação de pessoa jurídica para prestação de serviços de locação, instalação e operação de equipamento tipo "GRID Box Truss e Portal" para utilização nos eventos do Município de Nilo Peçanha - BA., na forma estabelecida no Termo de Referência e de acordo com a proposta do contratado que para todos os efeitos integra este contrato como se transcrita fosse, apresentada na forma de anexo único ao presente.</t>
+        </is>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>PREFEITURA MUNICIPAL DE NILO PEÇANHA</t>
+        </is>
+      </c>
+      <c r="I51" t="inlineStr">
+        <is>
+          <t>56.400,00</t>
+        </is>
+      </c>
+      <c r="J51" t="inlineStr"/>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>067/2024</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>DV004/2024SEMAD</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>24 de maio de 2024</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>31 de dezembro de 2024</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>MARIA DE LOURDES MEIRELLES LISBOA DE BRITO, CNPJ 18.967.907/0001-90</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>DISPENSA DE LICITAÇÃO</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>Contratação de pessoa jurídica para prestação de serviços de locação, instalação e operação de equipamento tipo "GRID Box Truss e Portal" para utilização nos eventos do Município de Nilo Peçanha - BA., na forma estabelecida no Termo de Referência e de acordo com a proposta do contratado que para todos os efeitos integra este contrato como se transcrita fosse, apresentada na forma de anexo único ao presente.</t>
+        </is>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>PREFEITURA MUNICIPAL DE NILO PEÇANHA</t>
+        </is>
+      </c>
+      <c r="I52" t="inlineStr">
+        <is>
+          <t>R$ 56.400,00 (cinquenta e seis mil e quatrocentos reais)</t>
+        </is>
+      </c>
+      <c r="J52" t="inlineStr"/>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>091/2023</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>Não informado</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>01 de agosto de 2023</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>Não informado</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>POSITIVO TECNOLOGIA S.A., CNPJ 81.243.735/0001-48</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>Inexigibilidade</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>Aquisição de central educacional alfabeto e upgrade e-blocks matemática que promoverá a inclusão dos alunos do município de Nilo Peçanha-Ba, contendo o serviço de instalação e formação de educadores, conforme especificações descritas na proposta comercial.</t>
+        </is>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>FUNDO MUNICIPAL DE EDUCAÇÃO</t>
+        </is>
+      </c>
+      <c r="I53" t="inlineStr">
+        <is>
+          <t>R$175.334,00 (Cento e setenta e cinco mil trezentos e trinta e quatro reais)</t>
+        </is>
+      </c>
+      <c r="J53" t="inlineStr"/>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>091/2023</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Não informado</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>01 de agosto de 2023</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>Não informado</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>POSITIVO TECNOLOGIA S.A., CNPJ 81.243.735/0001-48</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>Inexigibilidade</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>Aquisição de central educacional alfabeto e upgrade e-blocks matemática que promoverá a inclusão dos alunos do município de Nilo Peçanha-Ba, contendo o serviço de instalação e formação de educadores, conforme especificações descritas na proposta comercial.</t>
+        </is>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>FUNDO MUNICIPAL DE EDUCAÇÃO</t>
+        </is>
+      </c>
+      <c r="I54" t="inlineStr">
+        <is>
+          <t>R$175.334,00 (Cento e setenta e cinco mil trezentos e trinta e quatro reais)</t>
+        </is>
+      </c>
+      <c r="J54" t="inlineStr"/>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>091/2023</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Não informado</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>01 de agosto de 2023</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>Não informado</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>POSITIVO TECNOLOGIA S.A., CNPJ 81.243.735/0001-48</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>Inexigibilidade nº 033/2023</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>Aquisição de central educacional alfabeto e upgrade e-blocks matemática que promoverá a inclusão dos alunos do município de Nilo Peçanha-Ba, contendo o serviço de instalação e formação de educadores, conforme especificações descritas na proposta comercial.</t>
+        </is>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>FUNDO MUNICIPAL DE EDUCAÇÃO</t>
+        </is>
+      </c>
+      <c r="I55" t="inlineStr">
+        <is>
+          <t>R$175.334,00 (Cento e setenta e cinco mil trezentos e trinta e quatro reais)</t>
+        </is>
+      </c>
+      <c r="J55" t="inlineStr"/>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>091/2023</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>033/2023</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>01 de agosto de 2023</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>Não informado</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>POSITIVO TECNOLOGIA S.A., CNPJ 81.243.735/0001-48</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>Inexigibilidade</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>Aquisição de central educacional alfabeto e upgrade e-blocks matemática que promoverá a inclusão dos alunos do município de Nilo Peçanha-Ba, contendo o serviço de instalação e formação de educadores, conforme especificações descritas na proposta comercial.</t>
+        </is>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>FUNDO MUNICIPAL DE EDUCAÇÃO</t>
+        </is>
+      </c>
+      <c r="I56" t="inlineStr">
+        <is>
+          <t>R$175.334,00 (Cento e setenta e cinco mil trezentos e trinta e quatro reais)</t>
+        </is>
+      </c>
+      <c r="J56" t="inlineStr"/>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>091/2023</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>033/2023</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>01 de agosto de 2023</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>Não informado</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>POSITIVO TECNOLOGIA S.A., CNPJ 81.243.735/0001-48</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Inexigibilidade </t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>Aquisição de central educacional alfabeto e upgrade e-blocks matemática que promoverá a inclusão dos alunos do município de Nilo Peçanha-Ba, contendo o serviço de instalação e formação de educadores, conforme especificações descritas na proposta comercial.</t>
+        </is>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>FUNDO MUNICIPAL DE EDUCAÇÃO</t>
+        </is>
+      </c>
+      <c r="I57" t="inlineStr">
+        <is>
+          <t>R$175.334,00 (Cento e setenta e cinco mil trezentos e trinta e quatro reais)</t>
+        </is>
+      </c>
+      <c r="J57" t="inlineStr"/>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>091/2023</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>033/2023</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>01 de agosto de 2023</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>Não informado</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>POSITIVO TECNOLOGIA S.A., CNPJ 81.243.735/0001-48</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Inexigibilidade </t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>Aquisição de central educacional alfabeto e upgrade e-blocks matemática que promoverá a inclusão dos alunos do município de Nilo Peçanha-Ba, contendo o serviço de instalação e formação de educadores, conforme especificações descritas na proposta comercial.</t>
+        </is>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>FUNDO MUNICIPAL DE EDUCAÇÃO</t>
+        </is>
+      </c>
+      <c r="I58" t="inlineStr">
+        <is>
+          <t>R$175.334,00 (Cento e setenta e cinco mil trezentos e trinta e quatro reais)</t>
+        </is>
+      </c>
+      <c r="J58" t="inlineStr"/>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>091/2023</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>033/2023</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>01 de agosto de 2023</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>Não informado</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>POSITIVO TECNOLOGIA S.A., CNPJ 81.243.735/0001-48</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Inexigibilidade </t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>Aquisição de central educacional alfabeto e upgrade e-blocks matemática que promoverá a inclusão dos alunos do município de Nilo Peçanha-Ba, contendo o serviço de instalação e formação de educadores</t>
+        </is>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>FUNDO MUNICIPAL DE EDUCAÇÃO</t>
+        </is>
+      </c>
+      <c r="I59" t="inlineStr">
+        <is>
+          <t>R$175.334,00 (Cento e setenta e cinco mil trezentos e trinta e quatro reais)</t>
+        </is>
+      </c>
+      <c r="J59" t="inlineStr"/>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>091/2023</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>033/2023</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>01 de agosto de 2023</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>Não informado</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>POSITIVO TECNOLOGIA S.A., CNPJ 81.243.735/0001-48</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Inexigibilidade </t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>Aquisição de central educacional alfabeto e upgrade e-blocks matemática que promoverá a inclusão dos alunos do município de Nilo Peçanha-Ba, contendo o serviço de instalação e formação de educadores, conforme especificações descritas na proposta comercial.</t>
+        </is>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>FUNDO MUNICIPAL DE EDUCAÇÃO</t>
+        </is>
+      </c>
+      <c r="I60" t="inlineStr">
+        <is>
+          <t>R$175.334,00 (Cento e setenta e cinco mil trezentos e trinta e quatro reais)</t>
+        </is>
+      </c>
+      <c r="J60" t="inlineStr"/>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>091/2023</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>033/2023</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>01 de agosto de 2023</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>Não informado</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>POSITIVO TECNOLOGIA S.A., CNPJ 81.243.735/0001-48</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>Inexigibilidade</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>Aquisição de central educacional alfabeto e upgrade e-blocks matemática que promoverá a inclusão dos alunos do município de Nilo Peçanha-Ba, contendo o serviço de instalação e formação de educadores, conforme especificações descritas na proposta comercial.</t>
+        </is>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>FUNDO MUNICIPAL DE EDUCAÇÃO</t>
+        </is>
+      </c>
+      <c r="I61" t="inlineStr">
+        <is>
+          <t>R$175.334,00 (Cento e setenta e cinco mil trezentos e trinta e quatro reais).</t>
+        </is>
+      </c>
+      <c r="J61" t="inlineStr"/>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>091/2023</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>033/2023</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>01 de agosto de 2023</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>Não informado</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>POSITIVO TECNOLOGIA S.A., CNPJ 81.243.735/0001-48</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Inexigibilidade </t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>Aquisição de central educacional alfabeto e upgrade e-blocks matemática que promoverá a inclusão dos alunos do município de Nilo Peçanha-Ba, contendo o serviço de instalação e formação de educadores, conforme especificações descritas na proposta comercial.</t>
+        </is>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>FUNDO MUNICIPAL DE EDUCAÇÃO</t>
+        </is>
+      </c>
+      <c r="I62" t="inlineStr">
+        <is>
+          <t>R$175.334,00 (Cento e setenta e cinco mil trezentos e trinta e quatro reais)</t>
+        </is>
+      </c>
+      <c r="J62" t="inlineStr"/>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>143/2023</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>003/2023</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>06 de novembro de 2023</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>Não informado</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>COOPERATIVA AGRÍCOLA DE
+DESENVOLVIMENTO SUSTENTÁVEL DO SUL DA BAHIA (grupo formal), CNPJ 28.716.605/0001-00</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>Chamada Pública</t>
+        </is>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>AQUISIÇÃO DE GÊNEROS
+ALIMENTÍCIOS PARA ATENDIMENTO AO
+PROGRAMA NACIONAL DE ALIMENTAÇÃO
+ESCOLAR - PNAE</t>
+        </is>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>FUNDO MUNICIPAL DE EDUCAÇÃO</t>
+        </is>
+      </c>
+      <c r="I63" t="inlineStr">
+        <is>
+          <t>R$59.520,00
+(cinquenta nove mil, quinhentos vinte reais)</t>
+        </is>
+      </c>
+      <c r="J63" t="inlineStr"/>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>099/2023</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>003/2023</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>25 de agosto de 2023</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>Não informado</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>MARIA JOVENCI SANTOS GOMES (fornecedor individual),  inscrito no CPF sob o n°. 188.930.665-72</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>Chamada Pública</t>
+        </is>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>AQUISIÇÃO DE GÊNEROS
+ALIMENTÍCIOS PARA ATENDIMENTO AO
+PROGRAMA NACIONAL DE ALIMENTAÇÃO
+ESCOLAR - PNAE</t>
+        </is>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>FUNDO MUNICIPAL DE EDUCAÇÃO</t>
+        </is>
+      </c>
+      <c r="I64" t="inlineStr">
+        <is>
+          <t>R$20.565,50 (vinte mil
+e quinhentos sessenta cinco reais e cinquenta centavos)</t>
+        </is>
+      </c>
+      <c r="J64" t="inlineStr"/>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>099/2023</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>Não informado</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>25 de agosto de 2023</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>Não informado</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>MARIA JOVENCI SANTOS GOMES (fornecedor individual),  inscrito no CPF sob o n°. 188.930.665-72</t>
+        </is>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>Chamada Pública</t>
+        </is>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>AQUISIÇÃO DE GÊNEROS
+ALIMENTÍCIOS PARA ATENDIMENTO AO
+PROGRAMA NACIONAL DE ALIMENTAÇÃO
+ESCOLAR - PNAE</t>
+        </is>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>FUNDO MUNICIPAL DE EDUCAÇÃO</t>
+        </is>
+      </c>
+      <c r="I65" t="inlineStr">
+        <is>
+          <t>R$20.565,50 (vinte mil
+e quinhentos sessenta cinco reais e cinquenta centavos)</t>
+        </is>
+      </c>
+      <c r="J65" t="inlineStr"/>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>093/2023</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>06/2023</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>09 de agosto de 2023</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>Não informado</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>PLENA PROJETOS DE PLAYGROUNDS E BRINQUEDOS EIRELI, CNPJ 28.167.794/0001-00</t>
+        </is>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>Pregão Eletrônico</t>
+        </is>
+      </c>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>fornecimento de playgrounds para atender as necessidades da Secretaria de Educação do Município de Nilo Peçanha/Ba.</t>
+        </is>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>FUNDO MUNICIPAL DE EDUCAÇÃO</t>
+        </is>
+      </c>
+      <c r="I66" t="inlineStr">
+        <is>
+          <t>R$89.050,00 (oitenta e nove mil e cinquenta reais)</t>
+        </is>
+      </c>
+      <c r="J66" t="inlineStr"/>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>093/2023</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>06/2023</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>09 de agosto de 2023</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>Não informado</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>PLENA PROJETOS DE PLAYGROUNDS E BRINQUEDOS EIRELI, CNPJ 28.167.794/0001-00</t>
+        </is>
+      </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>Pregão Eletrônico</t>
+        </is>
+      </c>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>fornecimento de playgrounds para atender as necessidades da Secretaria de Educação do Município de Nilo Peçanha/Ba.</t>
+        </is>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>PREFEITURA MUNICIPAL DE NILO PEÇANHA / FUNDO MUNICIPAL DE EDUCAÇÃO DE NILO PEÇANHA - BAHIA</t>
+        </is>
+      </c>
+      <c r="I67" t="inlineStr">
+        <is>
+          <t>R$89.050,00 (oitenta e nove mil e cinquenta reais)</t>
+        </is>
+      </c>
+      <c r="J67" t="inlineStr"/>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>091/2023</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>Não informado</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>01 de agosto de 2023</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>Não informado</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>POSITIVO TECNOLOGIA S.A.</t>
+        </is>
+      </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>Inexigibilidade nº 033/2023</t>
+        </is>
+      </c>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>Aquisição de central educacional alfabeto e upgrade e-blocks matemática que promoverá a inclusão dos alunos do município de Nilo Peçanha-Ba, contendo o serviço de instalação e formação de educadores, conforme especificações descritas na proposta comercial.</t>
+        </is>
+      </c>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>FUNDO MUNICIPAL DE EDUCAÇÃO</t>
+        </is>
+      </c>
+      <c r="I68" t="inlineStr">
+        <is>
+          <t>R$175.334,00 (Cento e setenta e cinco mil trezentos e trinta e quatro reais)</t>
+        </is>
+      </c>
+      <c r="J68" t="inlineStr">
+        <is>
+          <t>81.243.735/0001-48</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>067/2024</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>DV004/2024SEMAD</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>24 de maio de 2024</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>31 de dezembro de 2024</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>MARIA DE LOURDES MEIRELLES LISBOA DE BRITO</t>
+        </is>
+      </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>DISPENSA DE LICITAÇÃO</t>
+        </is>
+      </c>
+      <c r="G69" t="inlineStr">
+        <is>
+          <t>Contratação de pessoa jurídica para prestação de serviços de locação, instalação e operação de equipamento tipo "GRID Box Truss e Portal" para utilização nos eventos do Município de Nilo Peçanha - BA.</t>
+        </is>
+      </c>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>PREFEITURA MUNICIPAL DE NILO PEÇANHA</t>
+        </is>
+      </c>
+      <c r="I69" t="inlineStr">
+        <is>
+          <t>R$ 56.400,00</t>
+        </is>
+      </c>
+      <c r="J69" t="inlineStr">
+        <is>
+          <t>18.967.907/0001-90</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>067/2024</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>DV004/2024SEMAD</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>24 de maio de 2024</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>31 de dezembro de 2024</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>MARIA DE LOURDES MEIRELLES LISBOA DE BRITO</t>
+        </is>
+      </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>DISPENSA DE LICITAÇÃO</t>
+        </is>
+      </c>
+      <c r="G70" t="inlineStr">
+        <is>
+          <t>Contratação de pessoa jurídica para prestação de serviços de locação, instalação e operação de equipamento tipo "GRID Box Truss e Portal" para utilização nos eventos do Município de Nilo Peçanha - BA.</t>
+        </is>
+      </c>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>PREFEITURA MUNICIPAL DE NILO PEÇANHA</t>
+        </is>
+      </c>
+      <c r="I70" t="inlineStr">
+        <is>
+          <t>R$ 56.400,00</t>
+        </is>
+      </c>
+      <c r="J70" t="inlineStr">
+        <is>
+          <t>18.967.907/0001-90</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>067/2024</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>DV004/2024SEMAD</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>24 de maio de 2024</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>31 de dezembro de 2024</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>MARIA DE LOURDES MEIRELLES LISBOA DE BRITO</t>
+        </is>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>DISPENSA DE LICITAÇÃO</t>
+        </is>
+      </c>
+      <c r="G71" t="inlineStr">
+        <is>
+          <t>Contratação de pessoa jurídica para prestação de serviços de locação, instalação e operação de equipamento tipo "GRID Box Truss e Portal" para utilização nos eventos do Município de Nilo Peçanha - BA.</t>
+        </is>
+      </c>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t>PREFEITURA MUNICIPAL DE NILO PEÇANHA</t>
+        </is>
+      </c>
+      <c r="I71" t="inlineStr">
+        <is>
+          <t>R$ 56.400,00</t>
+        </is>
+      </c>
+      <c r="J71" t="inlineStr">
+        <is>
+          <t>18.967.907/0001-90</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>067/2024</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>DV004/2024SEMAD</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>24 de maio de 2024</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>31 de dezembro de 2024</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>MARIA DE LOURDES MEIRELLES LISBOA DE BRITO</t>
+        </is>
+      </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>DISPENSA DE LICITAÇÃO</t>
+        </is>
+      </c>
+      <c r="G72" t="inlineStr">
+        <is>
+          <t>Contratação de pessoa jurídica para prestação de serviços de locação, instalação e operação de equipamento tipo "GRID Box Truss e Portal" para utilização nos eventos do Município de Nilo Peçanha - BA.</t>
+        </is>
+      </c>
+      <c r="H72" t="inlineStr">
+        <is>
+          <t>MUNICÍPIO DE NILO PEÇANHA</t>
+        </is>
+      </c>
+      <c r="I72" t="inlineStr">
+        <is>
+          <t>56.400,00</t>
+        </is>
+      </c>
+      <c r="J72" t="inlineStr">
+        <is>
+          <t>18.967.907/0001-90</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
fix invalid response genail check, and casting int to port number
</commit_message>
<xml_diff>
--- a/contratos.xlsx
+++ b/contratos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J72"/>
+  <dimension ref="A1:U73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -484,6 +484,61 @@
           <t>CNPJ</t>
         </is>
       </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>n_contrato</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>n_licitacao</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>assinatura</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>vencimento</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>contratada</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>cnpj</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>modalidade</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>objeto</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>contratante</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>valor</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>filename</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -532,6 +587,17 @@
         </is>
       </c>
       <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr"/>
+      <c r="M2" t="inlineStr"/>
+      <c r="N2" t="inlineStr"/>
+      <c r="O2" t="inlineStr"/>
+      <c r="P2" t="inlineStr"/>
+      <c r="Q2" t="inlineStr"/>
+      <c r="R2" t="inlineStr"/>
+      <c r="S2" t="inlineStr"/>
+      <c r="T2" t="inlineStr"/>
+      <c r="U2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -580,6 +646,17 @@
         </is>
       </c>
       <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr"/>
+      <c r="P3" t="inlineStr"/>
+      <c r="Q3" t="inlineStr"/>
+      <c r="R3" t="inlineStr"/>
+      <c r="S3" t="inlineStr"/>
+      <c r="T3" t="inlineStr"/>
+      <c r="U3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -628,6 +705,17 @@
         </is>
       </c>
       <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr"/>
+      <c r="O4" t="inlineStr"/>
+      <c r="P4" t="inlineStr"/>
+      <c r="Q4" t="inlineStr"/>
+      <c r="R4" t="inlineStr"/>
+      <c r="S4" t="inlineStr"/>
+      <c r="T4" t="inlineStr"/>
+      <c r="U4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -676,6 +764,17 @@
         </is>
       </c>
       <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr"/>
+      <c r="M5" t="inlineStr"/>
+      <c r="N5" t="inlineStr"/>
+      <c r="O5" t="inlineStr"/>
+      <c r="P5" t="inlineStr"/>
+      <c r="Q5" t="inlineStr"/>
+      <c r="R5" t="inlineStr"/>
+      <c r="S5" t="inlineStr"/>
+      <c r="T5" t="inlineStr"/>
+      <c r="U5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -724,6 +823,17 @@
         </is>
       </c>
       <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
+      <c r="L6" t="inlineStr"/>
+      <c r="M6" t="inlineStr"/>
+      <c r="N6" t="inlineStr"/>
+      <c r="O6" t="inlineStr"/>
+      <c r="P6" t="inlineStr"/>
+      <c r="Q6" t="inlineStr"/>
+      <c r="R6" t="inlineStr"/>
+      <c r="S6" t="inlineStr"/>
+      <c r="T6" t="inlineStr"/>
+      <c r="U6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -772,6 +882,17 @@
         </is>
       </c>
       <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr"/>
+      <c r="L7" t="inlineStr"/>
+      <c r="M7" t="inlineStr"/>
+      <c r="N7" t="inlineStr"/>
+      <c r="O7" t="inlineStr"/>
+      <c r="P7" t="inlineStr"/>
+      <c r="Q7" t="inlineStr"/>
+      <c r="R7" t="inlineStr"/>
+      <c r="S7" t="inlineStr"/>
+      <c r="T7" t="inlineStr"/>
+      <c r="U7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -820,6 +941,17 @@
         </is>
       </c>
       <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
+      <c r="L8" t="inlineStr"/>
+      <c r="M8" t="inlineStr"/>
+      <c r="N8" t="inlineStr"/>
+      <c r="O8" t="inlineStr"/>
+      <c r="P8" t="inlineStr"/>
+      <c r="Q8" t="inlineStr"/>
+      <c r="R8" t="inlineStr"/>
+      <c r="S8" t="inlineStr"/>
+      <c r="T8" t="inlineStr"/>
+      <c r="U8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -868,6 +1000,17 @@
         </is>
       </c>
       <c r="J9" t="inlineStr"/>
+      <c r="K9" t="inlineStr"/>
+      <c r="L9" t="inlineStr"/>
+      <c r="M9" t="inlineStr"/>
+      <c r="N9" t="inlineStr"/>
+      <c r="O9" t="inlineStr"/>
+      <c r="P9" t="inlineStr"/>
+      <c r="Q9" t="inlineStr"/>
+      <c r="R9" t="inlineStr"/>
+      <c r="S9" t="inlineStr"/>
+      <c r="T9" t="inlineStr"/>
+      <c r="U9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -916,6 +1059,17 @@
         </is>
       </c>
       <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="inlineStr"/>
+      <c r="M10" t="inlineStr"/>
+      <c r="N10" t="inlineStr"/>
+      <c r="O10" t="inlineStr"/>
+      <c r="P10" t="inlineStr"/>
+      <c r="Q10" t="inlineStr"/>
+      <c r="R10" t="inlineStr"/>
+      <c r="S10" t="inlineStr"/>
+      <c r="T10" t="inlineStr"/>
+      <c r="U10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -964,6 +1118,17 @@
         </is>
       </c>
       <c r="J11" t="inlineStr"/>
+      <c r="K11" t="inlineStr"/>
+      <c r="L11" t="inlineStr"/>
+      <c r="M11" t="inlineStr"/>
+      <c r="N11" t="inlineStr"/>
+      <c r="O11" t="inlineStr"/>
+      <c r="P11" t="inlineStr"/>
+      <c r="Q11" t="inlineStr"/>
+      <c r="R11" t="inlineStr"/>
+      <c r="S11" t="inlineStr"/>
+      <c r="T11" t="inlineStr"/>
+      <c r="U11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1012,6 +1177,17 @@
         </is>
       </c>
       <c r="J12" t="inlineStr"/>
+      <c r="K12" t="inlineStr"/>
+      <c r="L12" t="inlineStr"/>
+      <c r="M12" t="inlineStr"/>
+      <c r="N12" t="inlineStr"/>
+      <c r="O12" t="inlineStr"/>
+      <c r="P12" t="inlineStr"/>
+      <c r="Q12" t="inlineStr"/>
+      <c r="R12" t="inlineStr"/>
+      <c r="S12" t="inlineStr"/>
+      <c r="T12" t="inlineStr"/>
+      <c r="U12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1060,6 +1236,17 @@
         </is>
       </c>
       <c r="J13" t="inlineStr"/>
+      <c r="K13" t="inlineStr"/>
+      <c r="L13" t="inlineStr"/>
+      <c r="M13" t="inlineStr"/>
+      <c r="N13" t="inlineStr"/>
+      <c r="O13" t="inlineStr"/>
+      <c r="P13" t="inlineStr"/>
+      <c r="Q13" t="inlineStr"/>
+      <c r="R13" t="inlineStr"/>
+      <c r="S13" t="inlineStr"/>
+      <c r="T13" t="inlineStr"/>
+      <c r="U13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1108,6 +1295,17 @@
         </is>
       </c>
       <c r="J14" t="inlineStr"/>
+      <c r="K14" t="inlineStr"/>
+      <c r="L14" t="inlineStr"/>
+      <c r="M14" t="inlineStr"/>
+      <c r="N14" t="inlineStr"/>
+      <c r="O14" t="inlineStr"/>
+      <c r="P14" t="inlineStr"/>
+      <c r="Q14" t="inlineStr"/>
+      <c r="R14" t="inlineStr"/>
+      <c r="S14" t="inlineStr"/>
+      <c r="T14" t="inlineStr"/>
+      <c r="U14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1156,6 +1354,17 @@
         </is>
       </c>
       <c r="J15" t="inlineStr"/>
+      <c r="K15" t="inlineStr"/>
+      <c r="L15" t="inlineStr"/>
+      <c r="M15" t="inlineStr"/>
+      <c r="N15" t="inlineStr"/>
+      <c r="O15" t="inlineStr"/>
+      <c r="P15" t="inlineStr"/>
+      <c r="Q15" t="inlineStr"/>
+      <c r="R15" t="inlineStr"/>
+      <c r="S15" t="inlineStr"/>
+      <c r="T15" t="inlineStr"/>
+      <c r="U15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1204,6 +1413,17 @@
         </is>
       </c>
       <c r="J16" t="inlineStr"/>
+      <c r="K16" t="inlineStr"/>
+      <c r="L16" t="inlineStr"/>
+      <c r="M16" t="inlineStr"/>
+      <c r="N16" t="inlineStr"/>
+      <c r="O16" t="inlineStr"/>
+      <c r="P16" t="inlineStr"/>
+      <c r="Q16" t="inlineStr"/>
+      <c r="R16" t="inlineStr"/>
+      <c r="S16" t="inlineStr"/>
+      <c r="T16" t="inlineStr"/>
+      <c r="U16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1252,6 +1472,17 @@
         </is>
       </c>
       <c r="J17" t="inlineStr"/>
+      <c r="K17" t="inlineStr"/>
+      <c r="L17" t="inlineStr"/>
+      <c r="M17" t="inlineStr"/>
+      <c r="N17" t="inlineStr"/>
+      <c r="O17" t="inlineStr"/>
+      <c r="P17" t="inlineStr"/>
+      <c r="Q17" t="inlineStr"/>
+      <c r="R17" t="inlineStr"/>
+      <c r="S17" t="inlineStr"/>
+      <c r="T17" t="inlineStr"/>
+      <c r="U17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1300,6 +1531,17 @@
         </is>
       </c>
       <c r="J18" t="inlineStr"/>
+      <c r="K18" t="inlineStr"/>
+      <c r="L18" t="inlineStr"/>
+      <c r="M18" t="inlineStr"/>
+      <c r="N18" t="inlineStr"/>
+      <c r="O18" t="inlineStr"/>
+      <c r="P18" t="inlineStr"/>
+      <c r="Q18" t="inlineStr"/>
+      <c r="R18" t="inlineStr"/>
+      <c r="S18" t="inlineStr"/>
+      <c r="T18" t="inlineStr"/>
+      <c r="U18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1348,6 +1590,17 @@
         </is>
       </c>
       <c r="J19" t="inlineStr"/>
+      <c r="K19" t="inlineStr"/>
+      <c r="L19" t="inlineStr"/>
+      <c r="M19" t="inlineStr"/>
+      <c r="N19" t="inlineStr"/>
+      <c r="O19" t="inlineStr"/>
+      <c r="P19" t="inlineStr"/>
+      <c r="Q19" t="inlineStr"/>
+      <c r="R19" t="inlineStr"/>
+      <c r="S19" t="inlineStr"/>
+      <c r="T19" t="inlineStr"/>
+      <c r="U19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1396,6 +1649,17 @@
         </is>
       </c>
       <c r="J20" t="inlineStr"/>
+      <c r="K20" t="inlineStr"/>
+      <c r="L20" t="inlineStr"/>
+      <c r="M20" t="inlineStr"/>
+      <c r="N20" t="inlineStr"/>
+      <c r="O20" t="inlineStr"/>
+      <c r="P20" t="inlineStr"/>
+      <c r="Q20" t="inlineStr"/>
+      <c r="R20" t="inlineStr"/>
+      <c r="S20" t="inlineStr"/>
+      <c r="T20" t="inlineStr"/>
+      <c r="U20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1444,6 +1708,17 @@
         </is>
       </c>
       <c r="J21" t="inlineStr"/>
+      <c r="K21" t="inlineStr"/>
+      <c r="L21" t="inlineStr"/>
+      <c r="M21" t="inlineStr"/>
+      <c r="N21" t="inlineStr"/>
+      <c r="O21" t="inlineStr"/>
+      <c r="P21" t="inlineStr"/>
+      <c r="Q21" t="inlineStr"/>
+      <c r="R21" t="inlineStr"/>
+      <c r="S21" t="inlineStr"/>
+      <c r="T21" t="inlineStr"/>
+      <c r="U21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1492,6 +1767,17 @@
         </is>
       </c>
       <c r="J22" t="inlineStr"/>
+      <c r="K22" t="inlineStr"/>
+      <c r="L22" t="inlineStr"/>
+      <c r="M22" t="inlineStr"/>
+      <c r="N22" t="inlineStr"/>
+      <c r="O22" t="inlineStr"/>
+      <c r="P22" t="inlineStr"/>
+      <c r="Q22" t="inlineStr"/>
+      <c r="R22" t="inlineStr"/>
+      <c r="S22" t="inlineStr"/>
+      <c r="T22" t="inlineStr"/>
+      <c r="U22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1540,6 +1826,17 @@
         </is>
       </c>
       <c r="J23" t="inlineStr"/>
+      <c r="K23" t="inlineStr"/>
+      <c r="L23" t="inlineStr"/>
+      <c r="M23" t="inlineStr"/>
+      <c r="N23" t="inlineStr"/>
+      <c r="O23" t="inlineStr"/>
+      <c r="P23" t="inlineStr"/>
+      <c r="Q23" t="inlineStr"/>
+      <c r="R23" t="inlineStr"/>
+      <c r="S23" t="inlineStr"/>
+      <c r="T23" t="inlineStr"/>
+      <c r="U23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1588,6 +1885,17 @@
         </is>
       </c>
       <c r="J24" t="inlineStr"/>
+      <c r="K24" t="inlineStr"/>
+      <c r="L24" t="inlineStr"/>
+      <c r="M24" t="inlineStr"/>
+      <c r="N24" t="inlineStr"/>
+      <c r="O24" t="inlineStr"/>
+      <c r="P24" t="inlineStr"/>
+      <c r="Q24" t="inlineStr"/>
+      <c r="R24" t="inlineStr"/>
+      <c r="S24" t="inlineStr"/>
+      <c r="T24" t="inlineStr"/>
+      <c r="U24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1636,6 +1944,17 @@
         </is>
       </c>
       <c r="J25" t="inlineStr"/>
+      <c r="K25" t="inlineStr"/>
+      <c r="L25" t="inlineStr"/>
+      <c r="M25" t="inlineStr"/>
+      <c r="N25" t="inlineStr"/>
+      <c r="O25" t="inlineStr"/>
+      <c r="P25" t="inlineStr"/>
+      <c r="Q25" t="inlineStr"/>
+      <c r="R25" t="inlineStr"/>
+      <c r="S25" t="inlineStr"/>
+      <c r="T25" t="inlineStr"/>
+      <c r="U25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1684,6 +2003,17 @@
         </is>
       </c>
       <c r="J26" t="inlineStr"/>
+      <c r="K26" t="inlineStr"/>
+      <c r="L26" t="inlineStr"/>
+      <c r="M26" t="inlineStr"/>
+      <c r="N26" t="inlineStr"/>
+      <c r="O26" t="inlineStr"/>
+      <c r="P26" t="inlineStr"/>
+      <c r="Q26" t="inlineStr"/>
+      <c r="R26" t="inlineStr"/>
+      <c r="S26" t="inlineStr"/>
+      <c r="T26" t="inlineStr"/>
+      <c r="U26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1732,6 +2062,17 @@
         </is>
       </c>
       <c r="J27" t="inlineStr"/>
+      <c r="K27" t="inlineStr"/>
+      <c r="L27" t="inlineStr"/>
+      <c r="M27" t="inlineStr"/>
+      <c r="N27" t="inlineStr"/>
+      <c r="O27" t="inlineStr"/>
+      <c r="P27" t="inlineStr"/>
+      <c r="Q27" t="inlineStr"/>
+      <c r="R27" t="inlineStr"/>
+      <c r="S27" t="inlineStr"/>
+      <c r="T27" t="inlineStr"/>
+      <c r="U27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1780,6 +2121,17 @@
         </is>
       </c>
       <c r="J28" t="inlineStr"/>
+      <c r="K28" t="inlineStr"/>
+      <c r="L28" t="inlineStr"/>
+      <c r="M28" t="inlineStr"/>
+      <c r="N28" t="inlineStr"/>
+      <c r="O28" t="inlineStr"/>
+      <c r="P28" t="inlineStr"/>
+      <c r="Q28" t="inlineStr"/>
+      <c r="R28" t="inlineStr"/>
+      <c r="S28" t="inlineStr"/>
+      <c r="T28" t="inlineStr"/>
+      <c r="U28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1828,6 +2180,17 @@
         </is>
       </c>
       <c r="J29" t="inlineStr"/>
+      <c r="K29" t="inlineStr"/>
+      <c r="L29" t="inlineStr"/>
+      <c r="M29" t="inlineStr"/>
+      <c r="N29" t="inlineStr"/>
+      <c r="O29" t="inlineStr"/>
+      <c r="P29" t="inlineStr"/>
+      <c r="Q29" t="inlineStr"/>
+      <c r="R29" t="inlineStr"/>
+      <c r="S29" t="inlineStr"/>
+      <c r="T29" t="inlineStr"/>
+      <c r="U29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1876,6 +2239,17 @@
         </is>
       </c>
       <c r="J30" t="inlineStr"/>
+      <c r="K30" t="inlineStr"/>
+      <c r="L30" t="inlineStr"/>
+      <c r="M30" t="inlineStr"/>
+      <c r="N30" t="inlineStr"/>
+      <c r="O30" t="inlineStr"/>
+      <c r="P30" t="inlineStr"/>
+      <c r="Q30" t="inlineStr"/>
+      <c r="R30" t="inlineStr"/>
+      <c r="S30" t="inlineStr"/>
+      <c r="T30" t="inlineStr"/>
+      <c r="U30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1924,6 +2298,17 @@
         </is>
       </c>
       <c r="J31" t="inlineStr"/>
+      <c r="K31" t="inlineStr"/>
+      <c r="L31" t="inlineStr"/>
+      <c r="M31" t="inlineStr"/>
+      <c r="N31" t="inlineStr"/>
+      <c r="O31" t="inlineStr"/>
+      <c r="P31" t="inlineStr"/>
+      <c r="Q31" t="inlineStr"/>
+      <c r="R31" t="inlineStr"/>
+      <c r="S31" t="inlineStr"/>
+      <c r="T31" t="inlineStr"/>
+      <c r="U31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -1972,6 +2357,17 @@
         </is>
       </c>
       <c r="J32" t="inlineStr"/>
+      <c r="K32" t="inlineStr"/>
+      <c r="L32" t="inlineStr"/>
+      <c r="M32" t="inlineStr"/>
+      <c r="N32" t="inlineStr"/>
+      <c r="O32" t="inlineStr"/>
+      <c r="P32" t="inlineStr"/>
+      <c r="Q32" t="inlineStr"/>
+      <c r="R32" t="inlineStr"/>
+      <c r="S32" t="inlineStr"/>
+      <c r="T32" t="inlineStr"/>
+      <c r="U32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -2020,6 +2416,17 @@
         </is>
       </c>
       <c r="J33" t="inlineStr"/>
+      <c r="K33" t="inlineStr"/>
+      <c r="L33" t="inlineStr"/>
+      <c r="M33" t="inlineStr"/>
+      <c r="N33" t="inlineStr"/>
+      <c r="O33" t="inlineStr"/>
+      <c r="P33" t="inlineStr"/>
+      <c r="Q33" t="inlineStr"/>
+      <c r="R33" t="inlineStr"/>
+      <c r="S33" t="inlineStr"/>
+      <c r="T33" t="inlineStr"/>
+      <c r="U33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -2068,6 +2475,17 @@
         </is>
       </c>
       <c r="J34" t="inlineStr"/>
+      <c r="K34" t="inlineStr"/>
+      <c r="L34" t="inlineStr"/>
+      <c r="M34" t="inlineStr"/>
+      <c r="N34" t="inlineStr"/>
+      <c r="O34" t="inlineStr"/>
+      <c r="P34" t="inlineStr"/>
+      <c r="Q34" t="inlineStr"/>
+      <c r="R34" t="inlineStr"/>
+      <c r="S34" t="inlineStr"/>
+      <c r="T34" t="inlineStr"/>
+      <c r="U34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -2116,6 +2534,17 @@
         </is>
       </c>
       <c r="J35" t="inlineStr"/>
+      <c r="K35" t="inlineStr"/>
+      <c r="L35" t="inlineStr"/>
+      <c r="M35" t="inlineStr"/>
+      <c r="N35" t="inlineStr"/>
+      <c r="O35" t="inlineStr"/>
+      <c r="P35" t="inlineStr"/>
+      <c r="Q35" t="inlineStr"/>
+      <c r="R35" t="inlineStr"/>
+      <c r="S35" t="inlineStr"/>
+      <c r="T35" t="inlineStr"/>
+      <c r="U35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -2164,6 +2593,17 @@
         </is>
       </c>
       <c r="J36" t="inlineStr"/>
+      <c r="K36" t="inlineStr"/>
+      <c r="L36" t="inlineStr"/>
+      <c r="M36" t="inlineStr"/>
+      <c r="N36" t="inlineStr"/>
+      <c r="O36" t="inlineStr"/>
+      <c r="P36" t="inlineStr"/>
+      <c r="Q36" t="inlineStr"/>
+      <c r="R36" t="inlineStr"/>
+      <c r="S36" t="inlineStr"/>
+      <c r="T36" t="inlineStr"/>
+      <c r="U36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -2212,6 +2652,17 @@
         </is>
       </c>
       <c r="J37" t="inlineStr"/>
+      <c r="K37" t="inlineStr"/>
+      <c r="L37" t="inlineStr"/>
+      <c r="M37" t="inlineStr"/>
+      <c r="N37" t="inlineStr"/>
+      <c r="O37" t="inlineStr"/>
+      <c r="P37" t="inlineStr"/>
+      <c r="Q37" t="inlineStr"/>
+      <c r="R37" t="inlineStr"/>
+      <c r="S37" t="inlineStr"/>
+      <c r="T37" t="inlineStr"/>
+      <c r="U37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -2260,6 +2711,17 @@
         </is>
       </c>
       <c r="J38" t="inlineStr"/>
+      <c r="K38" t="inlineStr"/>
+      <c r="L38" t="inlineStr"/>
+      <c r="M38" t="inlineStr"/>
+      <c r="N38" t="inlineStr"/>
+      <c r="O38" t="inlineStr"/>
+      <c r="P38" t="inlineStr"/>
+      <c r="Q38" t="inlineStr"/>
+      <c r="R38" t="inlineStr"/>
+      <c r="S38" t="inlineStr"/>
+      <c r="T38" t="inlineStr"/>
+      <c r="U38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -2308,6 +2770,17 @@
         </is>
       </c>
       <c r="J39" t="inlineStr"/>
+      <c r="K39" t="inlineStr"/>
+      <c r="L39" t="inlineStr"/>
+      <c r="M39" t="inlineStr"/>
+      <c r="N39" t="inlineStr"/>
+      <c r="O39" t="inlineStr"/>
+      <c r="P39" t="inlineStr"/>
+      <c r="Q39" t="inlineStr"/>
+      <c r="R39" t="inlineStr"/>
+      <c r="S39" t="inlineStr"/>
+      <c r="T39" t="inlineStr"/>
+      <c r="U39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -2356,6 +2829,17 @@
         </is>
       </c>
       <c r="J40" t="inlineStr"/>
+      <c r="K40" t="inlineStr"/>
+      <c r="L40" t="inlineStr"/>
+      <c r="M40" t="inlineStr"/>
+      <c r="N40" t="inlineStr"/>
+      <c r="O40" t="inlineStr"/>
+      <c r="P40" t="inlineStr"/>
+      <c r="Q40" t="inlineStr"/>
+      <c r="R40" t="inlineStr"/>
+      <c r="S40" t="inlineStr"/>
+      <c r="T40" t="inlineStr"/>
+      <c r="U40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -2404,6 +2888,17 @@
         </is>
       </c>
       <c r="J41" t="inlineStr"/>
+      <c r="K41" t="inlineStr"/>
+      <c r="L41" t="inlineStr"/>
+      <c r="M41" t="inlineStr"/>
+      <c r="N41" t="inlineStr"/>
+      <c r="O41" t="inlineStr"/>
+      <c r="P41" t="inlineStr"/>
+      <c r="Q41" t="inlineStr"/>
+      <c r="R41" t="inlineStr"/>
+      <c r="S41" t="inlineStr"/>
+      <c r="T41" t="inlineStr"/>
+      <c r="U41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -2452,6 +2947,17 @@
         </is>
       </c>
       <c r="J42" t="inlineStr"/>
+      <c r="K42" t="inlineStr"/>
+      <c r="L42" t="inlineStr"/>
+      <c r="M42" t="inlineStr"/>
+      <c r="N42" t="inlineStr"/>
+      <c r="O42" t="inlineStr"/>
+      <c r="P42" t="inlineStr"/>
+      <c r="Q42" t="inlineStr"/>
+      <c r="R42" t="inlineStr"/>
+      <c r="S42" t="inlineStr"/>
+      <c r="T42" t="inlineStr"/>
+      <c r="U42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -2500,6 +3006,17 @@
         </is>
       </c>
       <c r="J43" t="inlineStr"/>
+      <c r="K43" t="inlineStr"/>
+      <c r="L43" t="inlineStr"/>
+      <c r="M43" t="inlineStr"/>
+      <c r="N43" t="inlineStr"/>
+      <c r="O43" t="inlineStr"/>
+      <c r="P43" t="inlineStr"/>
+      <c r="Q43" t="inlineStr"/>
+      <c r="R43" t="inlineStr"/>
+      <c r="S43" t="inlineStr"/>
+      <c r="T43" t="inlineStr"/>
+      <c r="U43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -2548,6 +3065,17 @@
         </is>
       </c>
       <c r="J44" t="inlineStr"/>
+      <c r="K44" t="inlineStr"/>
+      <c r="L44" t="inlineStr"/>
+      <c r="M44" t="inlineStr"/>
+      <c r="N44" t="inlineStr"/>
+      <c r="O44" t="inlineStr"/>
+      <c r="P44" t="inlineStr"/>
+      <c r="Q44" t="inlineStr"/>
+      <c r="R44" t="inlineStr"/>
+      <c r="S44" t="inlineStr"/>
+      <c r="T44" t="inlineStr"/>
+      <c r="U44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -2596,6 +3124,17 @@
         </is>
       </c>
       <c r="J45" t="inlineStr"/>
+      <c r="K45" t="inlineStr"/>
+      <c r="L45" t="inlineStr"/>
+      <c r="M45" t="inlineStr"/>
+      <c r="N45" t="inlineStr"/>
+      <c r="O45" t="inlineStr"/>
+      <c r="P45" t="inlineStr"/>
+      <c r="Q45" t="inlineStr"/>
+      <c r="R45" t="inlineStr"/>
+      <c r="S45" t="inlineStr"/>
+      <c r="T45" t="inlineStr"/>
+      <c r="U45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -2644,6 +3183,17 @@
         </is>
       </c>
       <c r="J46" t="inlineStr"/>
+      <c r="K46" t="inlineStr"/>
+      <c r="L46" t="inlineStr"/>
+      <c r="M46" t="inlineStr"/>
+      <c r="N46" t="inlineStr"/>
+      <c r="O46" t="inlineStr"/>
+      <c r="P46" t="inlineStr"/>
+      <c r="Q46" t="inlineStr"/>
+      <c r="R46" t="inlineStr"/>
+      <c r="S46" t="inlineStr"/>
+      <c r="T46" t="inlineStr"/>
+      <c r="U46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -2692,6 +3242,17 @@
         </is>
       </c>
       <c r="J47" t="inlineStr"/>
+      <c r="K47" t="inlineStr"/>
+      <c r="L47" t="inlineStr"/>
+      <c r="M47" t="inlineStr"/>
+      <c r="N47" t="inlineStr"/>
+      <c r="O47" t="inlineStr"/>
+      <c r="P47" t="inlineStr"/>
+      <c r="Q47" t="inlineStr"/>
+      <c r="R47" t="inlineStr"/>
+      <c r="S47" t="inlineStr"/>
+      <c r="T47" t="inlineStr"/>
+      <c r="U47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -2740,6 +3301,17 @@
         </is>
       </c>
       <c r="J48" t="inlineStr"/>
+      <c r="K48" t="inlineStr"/>
+      <c r="L48" t="inlineStr"/>
+      <c r="M48" t="inlineStr"/>
+      <c r="N48" t="inlineStr"/>
+      <c r="O48" t="inlineStr"/>
+      <c r="P48" t="inlineStr"/>
+      <c r="Q48" t="inlineStr"/>
+      <c r="R48" t="inlineStr"/>
+      <c r="S48" t="inlineStr"/>
+      <c r="T48" t="inlineStr"/>
+      <c r="U48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -2788,6 +3360,17 @@
         </is>
       </c>
       <c r="J49" t="inlineStr"/>
+      <c r="K49" t="inlineStr"/>
+      <c r="L49" t="inlineStr"/>
+      <c r="M49" t="inlineStr"/>
+      <c r="N49" t="inlineStr"/>
+      <c r="O49" t="inlineStr"/>
+      <c r="P49" t="inlineStr"/>
+      <c r="Q49" t="inlineStr"/>
+      <c r="R49" t="inlineStr"/>
+      <c r="S49" t="inlineStr"/>
+      <c r="T49" t="inlineStr"/>
+      <c r="U49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -2836,6 +3419,17 @@
         </is>
       </c>
       <c r="J50" t="inlineStr"/>
+      <c r="K50" t="inlineStr"/>
+      <c r="L50" t="inlineStr"/>
+      <c r="M50" t="inlineStr"/>
+      <c r="N50" t="inlineStr"/>
+      <c r="O50" t="inlineStr"/>
+      <c r="P50" t="inlineStr"/>
+      <c r="Q50" t="inlineStr"/>
+      <c r="R50" t="inlineStr"/>
+      <c r="S50" t="inlineStr"/>
+      <c r="T50" t="inlineStr"/>
+      <c r="U50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -2884,6 +3478,17 @@
         </is>
       </c>
       <c r="J51" t="inlineStr"/>
+      <c r="K51" t="inlineStr"/>
+      <c r="L51" t="inlineStr"/>
+      <c r="M51" t="inlineStr"/>
+      <c r="N51" t="inlineStr"/>
+      <c r="O51" t="inlineStr"/>
+      <c r="P51" t="inlineStr"/>
+      <c r="Q51" t="inlineStr"/>
+      <c r="R51" t="inlineStr"/>
+      <c r="S51" t="inlineStr"/>
+      <c r="T51" t="inlineStr"/>
+      <c r="U51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -2932,6 +3537,17 @@
         </is>
       </c>
       <c r="J52" t="inlineStr"/>
+      <c r="K52" t="inlineStr"/>
+      <c r="L52" t="inlineStr"/>
+      <c r="M52" t="inlineStr"/>
+      <c r="N52" t="inlineStr"/>
+      <c r="O52" t="inlineStr"/>
+      <c r="P52" t="inlineStr"/>
+      <c r="Q52" t="inlineStr"/>
+      <c r="R52" t="inlineStr"/>
+      <c r="S52" t="inlineStr"/>
+      <c r="T52" t="inlineStr"/>
+      <c r="U52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -2980,6 +3596,17 @@
         </is>
       </c>
       <c r="J53" t="inlineStr"/>
+      <c r="K53" t="inlineStr"/>
+      <c r="L53" t="inlineStr"/>
+      <c r="M53" t="inlineStr"/>
+      <c r="N53" t="inlineStr"/>
+      <c r="O53" t="inlineStr"/>
+      <c r="P53" t="inlineStr"/>
+      <c r="Q53" t="inlineStr"/>
+      <c r="R53" t="inlineStr"/>
+      <c r="S53" t="inlineStr"/>
+      <c r="T53" t="inlineStr"/>
+      <c r="U53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -3028,6 +3655,17 @@
         </is>
       </c>
       <c r="J54" t="inlineStr"/>
+      <c r="K54" t="inlineStr"/>
+      <c r="L54" t="inlineStr"/>
+      <c r="M54" t="inlineStr"/>
+      <c r="N54" t="inlineStr"/>
+      <c r="O54" t="inlineStr"/>
+      <c r="P54" t="inlineStr"/>
+      <c r="Q54" t="inlineStr"/>
+      <c r="R54" t="inlineStr"/>
+      <c r="S54" t="inlineStr"/>
+      <c r="T54" t="inlineStr"/>
+      <c r="U54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -3076,6 +3714,17 @@
         </is>
       </c>
       <c r="J55" t="inlineStr"/>
+      <c r="K55" t="inlineStr"/>
+      <c r="L55" t="inlineStr"/>
+      <c r="M55" t="inlineStr"/>
+      <c r="N55" t="inlineStr"/>
+      <c r="O55" t="inlineStr"/>
+      <c r="P55" t="inlineStr"/>
+      <c r="Q55" t="inlineStr"/>
+      <c r="R55" t="inlineStr"/>
+      <c r="S55" t="inlineStr"/>
+      <c r="T55" t="inlineStr"/>
+      <c r="U55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -3124,6 +3773,17 @@
         </is>
       </c>
       <c r="J56" t="inlineStr"/>
+      <c r="K56" t="inlineStr"/>
+      <c r="L56" t="inlineStr"/>
+      <c r="M56" t="inlineStr"/>
+      <c r="N56" t="inlineStr"/>
+      <c r="O56" t="inlineStr"/>
+      <c r="P56" t="inlineStr"/>
+      <c r="Q56" t="inlineStr"/>
+      <c r="R56" t="inlineStr"/>
+      <c r="S56" t="inlineStr"/>
+      <c r="T56" t="inlineStr"/>
+      <c r="U56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -3172,6 +3832,17 @@
         </is>
       </c>
       <c r="J57" t="inlineStr"/>
+      <c r="K57" t="inlineStr"/>
+      <c r="L57" t="inlineStr"/>
+      <c r="M57" t="inlineStr"/>
+      <c r="N57" t="inlineStr"/>
+      <c r="O57" t="inlineStr"/>
+      <c r="P57" t="inlineStr"/>
+      <c r="Q57" t="inlineStr"/>
+      <c r="R57" t="inlineStr"/>
+      <c r="S57" t="inlineStr"/>
+      <c r="T57" t="inlineStr"/>
+      <c r="U57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -3220,6 +3891,17 @@
         </is>
       </c>
       <c r="J58" t="inlineStr"/>
+      <c r="K58" t="inlineStr"/>
+      <c r="L58" t="inlineStr"/>
+      <c r="M58" t="inlineStr"/>
+      <c r="N58" t="inlineStr"/>
+      <c r="O58" t="inlineStr"/>
+      <c r="P58" t="inlineStr"/>
+      <c r="Q58" t="inlineStr"/>
+      <c r="R58" t="inlineStr"/>
+      <c r="S58" t="inlineStr"/>
+      <c r="T58" t="inlineStr"/>
+      <c r="U58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -3268,6 +3950,17 @@
         </is>
       </c>
       <c r="J59" t="inlineStr"/>
+      <c r="K59" t="inlineStr"/>
+      <c r="L59" t="inlineStr"/>
+      <c r="M59" t="inlineStr"/>
+      <c r="N59" t="inlineStr"/>
+      <c r="O59" t="inlineStr"/>
+      <c r="P59" t="inlineStr"/>
+      <c r="Q59" t="inlineStr"/>
+      <c r="R59" t="inlineStr"/>
+      <c r="S59" t="inlineStr"/>
+      <c r="T59" t="inlineStr"/>
+      <c r="U59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -3316,6 +4009,17 @@
         </is>
       </c>
       <c r="J60" t="inlineStr"/>
+      <c r="K60" t="inlineStr"/>
+      <c r="L60" t="inlineStr"/>
+      <c r="M60" t="inlineStr"/>
+      <c r="N60" t="inlineStr"/>
+      <c r="O60" t="inlineStr"/>
+      <c r="P60" t="inlineStr"/>
+      <c r="Q60" t="inlineStr"/>
+      <c r="R60" t="inlineStr"/>
+      <c r="S60" t="inlineStr"/>
+      <c r="T60" t="inlineStr"/>
+      <c r="U60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -3364,6 +4068,17 @@
         </is>
       </c>
       <c r="J61" t="inlineStr"/>
+      <c r="K61" t="inlineStr"/>
+      <c r="L61" t="inlineStr"/>
+      <c r="M61" t="inlineStr"/>
+      <c r="N61" t="inlineStr"/>
+      <c r="O61" t="inlineStr"/>
+      <c r="P61" t="inlineStr"/>
+      <c r="Q61" t="inlineStr"/>
+      <c r="R61" t="inlineStr"/>
+      <c r="S61" t="inlineStr"/>
+      <c r="T61" t="inlineStr"/>
+      <c r="U61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -3412,6 +4127,17 @@
         </is>
       </c>
       <c r="J62" t="inlineStr"/>
+      <c r="K62" t="inlineStr"/>
+      <c r="L62" t="inlineStr"/>
+      <c r="M62" t="inlineStr"/>
+      <c r="N62" t="inlineStr"/>
+      <c r="O62" t="inlineStr"/>
+      <c r="P62" t="inlineStr"/>
+      <c r="Q62" t="inlineStr"/>
+      <c r="R62" t="inlineStr"/>
+      <c r="S62" t="inlineStr"/>
+      <c r="T62" t="inlineStr"/>
+      <c r="U62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -3465,6 +4191,17 @@
         </is>
       </c>
       <c r="J63" t="inlineStr"/>
+      <c r="K63" t="inlineStr"/>
+      <c r="L63" t="inlineStr"/>
+      <c r="M63" t="inlineStr"/>
+      <c r="N63" t="inlineStr"/>
+      <c r="O63" t="inlineStr"/>
+      <c r="P63" t="inlineStr"/>
+      <c r="Q63" t="inlineStr"/>
+      <c r="R63" t="inlineStr"/>
+      <c r="S63" t="inlineStr"/>
+      <c r="T63" t="inlineStr"/>
+      <c r="U63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -3517,6 +4254,17 @@
         </is>
       </c>
       <c r="J64" t="inlineStr"/>
+      <c r="K64" t="inlineStr"/>
+      <c r="L64" t="inlineStr"/>
+      <c r="M64" t="inlineStr"/>
+      <c r="N64" t="inlineStr"/>
+      <c r="O64" t="inlineStr"/>
+      <c r="P64" t="inlineStr"/>
+      <c r="Q64" t="inlineStr"/>
+      <c r="R64" t="inlineStr"/>
+      <c r="S64" t="inlineStr"/>
+      <c r="T64" t="inlineStr"/>
+      <c r="U64" t="inlineStr"/>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -3569,6 +4317,17 @@
         </is>
       </c>
       <c r="J65" t="inlineStr"/>
+      <c r="K65" t="inlineStr"/>
+      <c r="L65" t="inlineStr"/>
+      <c r="M65" t="inlineStr"/>
+      <c r="N65" t="inlineStr"/>
+      <c r="O65" t="inlineStr"/>
+      <c r="P65" t="inlineStr"/>
+      <c r="Q65" t="inlineStr"/>
+      <c r="R65" t="inlineStr"/>
+      <c r="S65" t="inlineStr"/>
+      <c r="T65" t="inlineStr"/>
+      <c r="U65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -3617,6 +4376,17 @@
         </is>
       </c>
       <c r="J66" t="inlineStr"/>
+      <c r="K66" t="inlineStr"/>
+      <c r="L66" t="inlineStr"/>
+      <c r="M66" t="inlineStr"/>
+      <c r="N66" t="inlineStr"/>
+      <c r="O66" t="inlineStr"/>
+      <c r="P66" t="inlineStr"/>
+      <c r="Q66" t="inlineStr"/>
+      <c r="R66" t="inlineStr"/>
+      <c r="S66" t="inlineStr"/>
+      <c r="T66" t="inlineStr"/>
+      <c r="U66" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -3665,6 +4435,17 @@
         </is>
       </c>
       <c r="J67" t="inlineStr"/>
+      <c r="K67" t="inlineStr"/>
+      <c r="L67" t="inlineStr"/>
+      <c r="M67" t="inlineStr"/>
+      <c r="N67" t="inlineStr"/>
+      <c r="O67" t="inlineStr"/>
+      <c r="P67" t="inlineStr"/>
+      <c r="Q67" t="inlineStr"/>
+      <c r="R67" t="inlineStr"/>
+      <c r="S67" t="inlineStr"/>
+      <c r="T67" t="inlineStr"/>
+      <c r="U67" t="inlineStr"/>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -3717,6 +4498,17 @@
           <t>81.243.735/0001-48</t>
         </is>
       </c>
+      <c r="K68" t="inlineStr"/>
+      <c r="L68" t="inlineStr"/>
+      <c r="M68" t="inlineStr"/>
+      <c r="N68" t="inlineStr"/>
+      <c r="O68" t="inlineStr"/>
+      <c r="P68" t="inlineStr"/>
+      <c r="Q68" t="inlineStr"/>
+      <c r="R68" t="inlineStr"/>
+      <c r="S68" t="inlineStr"/>
+      <c r="T68" t="inlineStr"/>
+      <c r="U68" t="inlineStr"/>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -3769,6 +4561,17 @@
           <t>18.967.907/0001-90</t>
         </is>
       </c>
+      <c r="K69" t="inlineStr"/>
+      <c r="L69" t="inlineStr"/>
+      <c r="M69" t="inlineStr"/>
+      <c r="N69" t="inlineStr"/>
+      <c r="O69" t="inlineStr"/>
+      <c r="P69" t="inlineStr"/>
+      <c r="Q69" t="inlineStr"/>
+      <c r="R69" t="inlineStr"/>
+      <c r="S69" t="inlineStr"/>
+      <c r="T69" t="inlineStr"/>
+      <c r="U69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -3821,6 +4624,17 @@
           <t>18.967.907/0001-90</t>
         </is>
       </c>
+      <c r="K70" t="inlineStr"/>
+      <c r="L70" t="inlineStr"/>
+      <c r="M70" t="inlineStr"/>
+      <c r="N70" t="inlineStr"/>
+      <c r="O70" t="inlineStr"/>
+      <c r="P70" t="inlineStr"/>
+      <c r="Q70" t="inlineStr"/>
+      <c r="R70" t="inlineStr"/>
+      <c r="S70" t="inlineStr"/>
+      <c r="T70" t="inlineStr"/>
+      <c r="U70" t="inlineStr"/>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -3873,6 +4687,17 @@
           <t>18.967.907/0001-90</t>
         </is>
       </c>
+      <c r="K71" t="inlineStr"/>
+      <c r="L71" t="inlineStr"/>
+      <c r="M71" t="inlineStr"/>
+      <c r="N71" t="inlineStr"/>
+      <c r="O71" t="inlineStr"/>
+      <c r="P71" t="inlineStr"/>
+      <c r="Q71" t="inlineStr"/>
+      <c r="R71" t="inlineStr"/>
+      <c r="S71" t="inlineStr"/>
+      <c r="T71" t="inlineStr"/>
+      <c r="U71" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -3925,6 +4750,80 @@
           <t>18.967.907/0001-90</t>
         </is>
       </c>
+      <c r="K72" t="inlineStr"/>
+      <c r="L72" t="inlineStr"/>
+      <c r="M72" t="inlineStr"/>
+      <c r="N72" t="inlineStr"/>
+      <c r="O72" t="inlineStr"/>
+      <c r="P72" t="inlineStr"/>
+      <c r="Q72" t="inlineStr"/>
+      <c r="R72" t="inlineStr"/>
+      <c r="S72" t="inlineStr"/>
+      <c r="T72" t="inlineStr"/>
+      <c r="U72" t="inlineStr"/>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr"/>
+      <c r="B73" t="inlineStr"/>
+      <c r="C73" t="inlineStr"/>
+      <c r="D73" t="inlineStr"/>
+      <c r="E73" t="inlineStr"/>
+      <c r="F73" t="inlineStr"/>
+      <c r="G73" t="inlineStr"/>
+      <c r="H73" t="inlineStr"/>
+      <c r="I73" t="inlineStr"/>
+      <c r="J73" t="inlineStr"/>
+      <c r="K73" t="inlineStr">
+        <is>
+          <t>154/2023</t>
+        </is>
+      </c>
+      <c r="L73" t="inlineStr">
+        <is>
+          <t>068/2023</t>
+        </is>
+      </c>
+      <c r="M73" t="inlineStr">
+        <is>
+          <t>19/12/2023</t>
+        </is>
+      </c>
+      <c r="N73" t="inlineStr">
+        <is>
+          <t>31/12/2023</t>
+        </is>
+      </c>
+      <c r="O73" t="inlineStr">
+        <is>
+          <t>LABORCOM COMÉRCIO DE MATERIAIS DE CONSTRUÇÃO LTDA.</t>
+        </is>
+      </c>
+      <c r="P73" t="inlineStr">
+        <is>
+          <t>34.101.659/0001-56</t>
+        </is>
+      </c>
+      <c r="Q73" t="inlineStr">
+        <is>
+          <t>DISPENSA DE LICITAÇÃO</t>
+        </is>
+      </c>
+      <c r="R73" t="inlineStr">
+        <is>
+          <t>Contratação de pessoa jurídica para fornecimento de material elétrico para ILUMINAÇÃO PÚBLICA em atendimento às necessidades da Secretaria de Infraestrutura e Urbanismo do Município de Nilo Peçanha - BA.</t>
+        </is>
+      </c>
+      <c r="S73" t="inlineStr">
+        <is>
+          <t>MUNICÍPIO DE NILO PEÇANHA</t>
+        </is>
+      </c>
+      <c r="T73" t="inlineStr">
+        <is>
+          <t>54.720,00</t>
+        </is>
+      </c>
+      <c r="U73" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
cutting tree similar senenteces of the bag of words
</commit_message>
<xml_diff>
--- a/contratos.xlsx
+++ b/contratos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U73"/>
+  <dimension ref="A1:U75"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4825,6 +4825,136 @@
       </c>
       <c r="U73" t="inlineStr"/>
     </row>
+    <row r="74">
+      <c r="A74" t="inlineStr"/>
+      <c r="B74" t="inlineStr"/>
+      <c r="C74" t="inlineStr"/>
+      <c r="D74" t="inlineStr"/>
+      <c r="E74" t="inlineStr"/>
+      <c r="F74" t="inlineStr"/>
+      <c r="G74" t="inlineStr"/>
+      <c r="H74" t="inlineStr"/>
+      <c r="I74" t="inlineStr"/>
+      <c r="J74" t="inlineStr"/>
+      <c r="K74" t="inlineStr">
+        <is>
+          <t>082/2024</t>
+        </is>
+      </c>
+      <c r="L74" t="inlineStr">
+        <is>
+          <t>IN020-2024SEMCULTE</t>
+        </is>
+      </c>
+      <c r="M74" t="inlineStr">
+        <is>
+          <t>27/06/2024</t>
+        </is>
+      </c>
+      <c r="N74" t="inlineStr">
+        <is>
+          <t>Não informado</t>
+        </is>
+      </c>
+      <c r="O74" t="inlineStr">
+        <is>
+          <t>Usina Mixx Produções LTDA</t>
+        </is>
+      </c>
+      <c r="P74" t="inlineStr">
+        <is>
+          <t>49.607.556/0001-30</t>
+        </is>
+      </c>
+      <c r="Q74" t="inlineStr">
+        <is>
+          <t>INEXIGIBILIDADE DE
+LICITAÇÃO</t>
+        </is>
+      </c>
+      <c r="R74" t="inlineStr">
+        <is>
+          <t>Contratação de pessoa jurídica para realização de
+show musical do(a) Artista MARLUS VIANA para apresentação nos Festejos de São Pedro 2024,
+no Município de Nilo Peçanha BA, conforme grade especificado pela Secretaria Municipal de
+Turismo, Cultura, Esporte e Lazer.</t>
+        </is>
+      </c>
+      <c r="S74" t="inlineStr">
+        <is>
+          <t>MUNICÍPIO DE NILO PEÇANHA</t>
+        </is>
+      </c>
+      <c r="T74" t="inlineStr">
+        <is>
+          <t>130.000,00</t>
+        </is>
+      </c>
+      <c r="U74" t="inlineStr"/>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr"/>
+      <c r="B75" t="inlineStr"/>
+      <c r="C75" t="inlineStr"/>
+      <c r="D75" t="inlineStr"/>
+      <c r="E75" t="inlineStr"/>
+      <c r="F75" t="inlineStr"/>
+      <c r="G75" t="inlineStr"/>
+      <c r="H75" t="inlineStr"/>
+      <c r="I75" t="inlineStr"/>
+      <c r="J75" t="inlineStr"/>
+      <c r="K75" t="inlineStr">
+        <is>
+          <t>154/2023</t>
+        </is>
+      </c>
+      <c r="L75" t="inlineStr">
+        <is>
+          <t>068/2023</t>
+        </is>
+      </c>
+      <c r="M75" t="inlineStr">
+        <is>
+          <t>19/12/2023</t>
+        </is>
+      </c>
+      <c r="N75" t="inlineStr">
+        <is>
+          <t>31/12/2023</t>
+        </is>
+      </c>
+      <c r="O75" t="inlineStr">
+        <is>
+          <t>LABORCOM COMÉRCIO DE MATERIAIS DE CONSTRUÇÃO LTDA.</t>
+        </is>
+      </c>
+      <c r="P75" t="inlineStr">
+        <is>
+          <t>34.101.659/0001-56</t>
+        </is>
+      </c>
+      <c r="Q75" t="inlineStr">
+        <is>
+          <t>DISPENSA DE LICITAÇÃO</t>
+        </is>
+      </c>
+      <c r="R75" t="inlineStr">
+        <is>
+          <t>Contratação de pessoa jurídica para fornecimento de material elétrico para ILUMINAÇÃO PÚBLICA em atendimento às necessidades da Secretaria de Infraestrutura e Urbanismo do Município de Nilo Peçanha - BA.</t>
+        </is>
+      </c>
+      <c r="S75" t="inlineStr">
+        <is>
+          <t>MUNICÍPIO DE NILO PEÇANHA</t>
+        </is>
+      </c>
+      <c r="T75" t="inlineStr">
+        <is>
+          <t>54.720,00</t>
+        </is>
+      </c>
+      <c r="U75" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
fix quads can be None
</commit_message>
<xml_diff>
--- a/contratos.xlsx
+++ b/contratos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U75"/>
+  <dimension ref="A1:U77"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4955,6 +4955,132 @@
       </c>
       <c r="U75" t="inlineStr"/>
     </row>
+    <row r="76">
+      <c r="A76" t="inlineStr"/>
+      <c r="B76" t="inlineStr"/>
+      <c r="C76" t="inlineStr"/>
+      <c r="D76" t="inlineStr"/>
+      <c r="E76" t="inlineStr"/>
+      <c r="F76" t="inlineStr"/>
+      <c r="G76" t="inlineStr"/>
+      <c r="H76" t="inlineStr"/>
+      <c r="I76" t="inlineStr"/>
+      <c r="J76" t="inlineStr"/>
+      <c r="K76" t="inlineStr">
+        <is>
+          <t>154/2023</t>
+        </is>
+      </c>
+      <c r="L76" t="inlineStr">
+        <is>
+          <t>068/2023</t>
+        </is>
+      </c>
+      <c r="M76" t="inlineStr">
+        <is>
+          <t>19/12/2023</t>
+        </is>
+      </c>
+      <c r="N76" t="inlineStr">
+        <is>
+          <t>31/12/2023</t>
+        </is>
+      </c>
+      <c r="O76" t="inlineStr">
+        <is>
+          <t>LABORCOM COMÉRCIO DE MATERIAIS DE CONSTRUÇÃO LTDA.</t>
+        </is>
+      </c>
+      <c r="P76" t="inlineStr">
+        <is>
+          <t>34.101.659/0001-56</t>
+        </is>
+      </c>
+      <c r="Q76" t="inlineStr">
+        <is>
+          <t>DISPENSA DE LICITAÇÃO</t>
+        </is>
+      </c>
+      <c r="R76" t="inlineStr">
+        <is>
+          <t>Contratação de pessoa jurídica para fornecimento de material elétrico para ILUMINAÇÃO PÚBLICA em atendimento às necessidades da Secretaria de Infraestrutura e Urbanismo do Município de Nilo Peçanha - BA., na forma estabelecida no Termo de Referência e de acordo com a proposta do contratado que para todos os efeitos integra este contrato como se transcrita fosse, apresentada na forma de anexo único ao presente.</t>
+        </is>
+      </c>
+      <c r="S76" t="inlineStr">
+        <is>
+          <t>MUNICÍPIO DE NILO PEÇANHA</t>
+        </is>
+      </c>
+      <c r="T76" t="inlineStr">
+        <is>
+          <t>54.720,00</t>
+        </is>
+      </c>
+      <c r="U76" t="inlineStr"/>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr"/>
+      <c r="B77" t="inlineStr"/>
+      <c r="C77" t="inlineStr"/>
+      <c r="D77" t="inlineStr"/>
+      <c r="E77" t="inlineStr"/>
+      <c r="F77" t="inlineStr"/>
+      <c r="G77" t="inlineStr"/>
+      <c r="H77" t="inlineStr"/>
+      <c r="I77" t="inlineStr"/>
+      <c r="J77" t="inlineStr"/>
+      <c r="K77" t="inlineStr">
+        <is>
+          <t>154/2023</t>
+        </is>
+      </c>
+      <c r="L77" t="inlineStr">
+        <is>
+          <t>068/2023</t>
+        </is>
+      </c>
+      <c r="M77" t="inlineStr">
+        <is>
+          <t>19/12/2023</t>
+        </is>
+      </c>
+      <c r="N77" t="inlineStr">
+        <is>
+          <t>31/12/2023</t>
+        </is>
+      </c>
+      <c r="O77" t="inlineStr">
+        <is>
+          <t>LABORCOM COMÉRCIO DE MATERIAIS DE CONSTRUÇÃO LTDA.</t>
+        </is>
+      </c>
+      <c r="P77" t="inlineStr">
+        <is>
+          <t>34.101.659/0001-56</t>
+        </is>
+      </c>
+      <c r="Q77" t="inlineStr">
+        <is>
+          <t>DISPENSA DE LICITAÇÃO</t>
+        </is>
+      </c>
+      <c r="R77" t="inlineStr">
+        <is>
+          <t>Contratação de pessoa jurídica para fornecimento de material elétrico para ILUMINAÇÃO PÚBLICA em atendimento às necessidades da Secretaria de Infraestrutura e Urbanismo do Município de Nilo Peçanha - BA., na forma estabelecida no Termo de Referência e de acordo com a proposta do contratado que para todos os efeitos integra este contrato como se transcrita fosse, apresentada na forma de anexo único ao presente.</t>
+        </is>
+      </c>
+      <c r="S77" t="inlineStr">
+        <is>
+          <t>MUNICÍPIO DE NILO PEÇANHA</t>
+        </is>
+      </c>
+      <c r="T77" t="inlineStr">
+        <is>
+          <t>54.720,00</t>
+        </is>
+      </c>
+      <c r="U77" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>